<commit_message>
changes on the self service side on personal laptop
</commit_message>
<xml_diff>
--- a/src/main/java/ExcelFiles/SelfService_ProspectInfo.xlsx
+++ b/src/main/java/ExcelFiles/SelfService_ProspectInfo.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{0C2FE70B-1E43-47B7-9795-BF98F101890F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="15045" windowHeight="11820" activeTab="1" xr2:uid="{01594B8C-F735-42A5-9305-EDA68BDBF78A}"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="15225" windowHeight="6555" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -13,7 +12,7 @@
     <sheet name="Applicant" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:J17"/>
+  <oleSize ref="B1:M20"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Email_ID</t>
   </si>
@@ -64,21 +63,6 @@
     <t>LegName</t>
   </si>
   <si>
-    <t>Undergraduate Calendar Type</t>
-  </si>
-  <si>
-    <t>Summer 2019</t>
-  </si>
-  <si>
-    <t>undergraduate Award</t>
-  </si>
-  <si>
-    <t>Nursing</t>
-  </si>
-  <si>
-    <t>Marketing</t>
-  </si>
-  <si>
     <t>FirstName</t>
   </si>
   <si>
@@ -100,37 +84,49 @@
     <t>Admitcode</t>
   </si>
   <si>
-    <t>Campus</t>
-  </si>
-  <si>
     <t>Residency</t>
   </si>
   <si>
     <t>Primarysource</t>
   </si>
   <si>
-    <t>Cross</t>
-  </si>
-  <si>
-    <t>Online</t>
-  </si>
-  <si>
     <t>On Campus</t>
   </si>
   <si>
-    <t>Adver - Radio</t>
-  </si>
-  <si>
-    <t>Automation140@mail.com</t>
-  </si>
-  <si>
-    <t>Automation167@mail.com</t>
+    <t>Automation1671@mail.com</t>
+  </si>
+  <si>
+    <t>PK CT</t>
+  </si>
+  <si>
+    <t>Spring 2020</t>
+  </si>
+  <si>
+    <t>PK Award</t>
+  </si>
+  <si>
+    <t>Business</t>
+  </si>
+  <si>
+    <t>Biology</t>
+  </si>
+  <si>
+    <t>Junio</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Event</t>
+  </si>
+  <si>
+    <t>testselfservice@mail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -235,7 +231,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -287,7 +283,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -481,18 +477,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22A3F7EB-90BE-4BD7-AAF0-6AC75A54B109}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -512,13 +508,13 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{06A2FB43-39DF-4049-88C4-FF8FE9EEE699}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{6046CCE3-7A67-4F1F-B919-72E3AF89FC0B}"/>
+    <hyperlink ref="A3" r:id="rId1"/>
+    <hyperlink ref="A2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
@@ -526,11 +522,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FA9F896-7295-4068-BBEB-B29DA594D68D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -584,37 +580,37 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" t="s">
+      <c r="G2" t="s">
         <v>14</v>
       </c>
-      <c r="C2" t="s">
+      <c r="H2" t="s">
         <v>15</v>
       </c>
-      <c r="D2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" t="s">
-        <v>20</v>
-      </c>
       <c r="I2" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="J2" t="s">
         <v>10</v>
       </c>
       <c r="K2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -624,52 +620,45 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{526BF666-6D2C-4ADD-8187-BAFD27C7A867}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E2" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>